<commit_message>
Adding event detection algorithms from CatEyes
</commit_message>
<xml_diff>
--- a/Counting C&Look DB.xlsx
+++ b/Counting C&Look DB.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucca\Desktop\Repositórios GitHub\CnLook_Clustering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repositories\CnLook_Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FF39B3-B2A3-42DF-BCFD-03DEF06C8D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679C25C2-A79C-4145-B0EA-27F995B80C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{3A05C7C3-5F9B-4051-AA72-D39C19BEA66A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3A05C7C3-5F9B-4051-AA72-D39C19BEA66A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="12" r:id="rId1"/>
-    <sheet name="Subjects" sheetId="13" r:id="rId2"/>
-    <sheet name="Planilha1" sheetId="14" r:id="rId3"/>
+    <sheet name="Tasks By ID" sheetId="15" r:id="rId2"/>
+    <sheet name="Subjects" sheetId="13" r:id="rId3"/>
+    <sheet name="Planilha1" sheetId="14" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -967,7 +968,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="301">
   <si>
     <t>Text: Golden_goose_1</t>
   </si>
@@ -1819,6 +1820,57 @@
   </si>
   <si>
     <t>Feature</t>
+  </si>
+  <si>
+    <t>Task Id</t>
+  </si>
+  <si>
+    <t>N_records</t>
+  </si>
+  <si>
+    <t>Task Names</t>
+  </si>
+  <si>
+    <t>"Horizontal" &amp; "Horizontal, 10 fixations"</t>
+  </si>
+  <si>
+    <t>"Horizontal2" &amp; "Horizontal2 Smooth"</t>
+  </si>
+  <si>
+    <t>"Reading: Two_letter_syllables_short" &amp; "Reading: Two_letter_syllables_short"</t>
+  </si>
+  <si>
+    <t>"Vertical"</t>
+  </si>
+  <si>
+    <t>"DiagonalLeftAndBack"</t>
+  </si>
+  <si>
+    <t>"DiagonalRightAndBack"</t>
+  </si>
+  <si>
+    <t>"Horizontal" &amp; "Horizontal Smooth"</t>
+  </si>
+  <si>
+    <t>"Easy_Swahili_Syllables"</t>
+  </si>
+  <si>
+    <t>"Horizontal"</t>
+  </si>
+  <si>
+    <t>"Vertical, 10 fixations"</t>
+  </si>
+  <si>
+    <t>"DiagonalRightAndBack, 10 fixations"</t>
+  </si>
+  <si>
+    <t>"DiagonalLeftAndBack, 10 fixations"</t>
+  </si>
+  <si>
+    <t>"DiagonalLeftAndBack Smooth"</t>
+  </si>
+  <si>
+    <t>"DiagonalRightAndBack Smooth"</t>
   </si>
 </sst>
 </file>
@@ -2165,7 +2217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2436,33 +2488,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2485,6 +2510,75 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3653,8 +3747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E63C6D2-241C-4155-9C99-E8FACD71DC3D}">
   <dimension ref="B4:AI133"/>
   <sheetViews>
-    <sheetView topLeftCell="W7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE30" sqref="AE30"/>
+    <sheetView topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK20" sqref="AK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3692,42 +3786,42 @@
     <row r="4" spans="2:35" ht="95.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F8" s="104" t="s">
+      <c r="F8" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="105"/>
-      <c r="H8" s="104" t="s">
+      <c r="G8" s="113"/>
+      <c r="H8" s="112" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="105"/>
-      <c r="J8" s="104" t="s">
+      <c r="I8" s="113"/>
+      <c r="J8" s="112" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="105"/>
-      <c r="L8" s="104" t="s">
+      <c r="K8" s="113"/>
+      <c r="L8" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="M8" s="105"/>
-      <c r="N8" s="104" t="s">
+      <c r="M8" s="113"/>
+      <c r="N8" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="O8" s="106"/>
-      <c r="P8" s="100" t="s">
+      <c r="O8" s="114"/>
+      <c r="P8" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="Q8" s="101"/>
-      <c r="R8" s="100" t="s">
+      <c r="Q8" s="111"/>
+      <c r="R8" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="S8" s="101"/>
-      <c r="T8" s="100" t="s">
+      <c r="S8" s="111"/>
+      <c r="T8" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="U8" s="102"/>
-      <c r="V8" s="100" t="s">
+      <c r="U8" s="110"/>
+      <c r="V8" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="W8" s="101"/>
+      <c r="W8" s="111"/>
     </row>
     <row r="9" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="51" t="s">
@@ -4136,13 +4230,13 @@
       <c r="W16" s="5"/>
       <c r="X16" s="14"/>
       <c r="Y16" s="14"/>
-      <c r="AF16" s="109">
+      <c r="AF16" s="100">
         <v>2515</v>
       </c>
       <c r="AG16" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="AH16" s="109">
+      <c r="AH16" s="100">
         <v>423</v>
       </c>
       <c r="AI16" s="14"/>
@@ -4182,13 +4276,13 @@
       <c r="W17" s="5"/>
       <c r="X17" s="14"/>
       <c r="Y17" s="14"/>
-      <c r="AF17" s="109">
+      <c r="AF17" s="100">
         <v>2511</v>
       </c>
       <c r="AG17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AH17" s="109">
+      <c r="AH17" s="100">
         <v>347</v>
       </c>
       <c r="AI17" s="14"/>
@@ -4236,13 +4330,13 @@
       <c r="W18" s="15"/>
       <c r="X18" s="14"/>
       <c r="Y18" s="14"/>
-      <c r="AF18" s="109">
+      <c r="AF18" s="100">
         <v>3218</v>
       </c>
       <c r="AG18" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="AH18" s="109">
+      <c r="AH18" s="100">
         <v>224</v>
       </c>
       <c r="AI18" s="14"/>
@@ -4298,13 +4392,13 @@
       </c>
       <c r="X19" s="14"/>
       <c r="Y19" s="14"/>
-      <c r="AF19" s="109">
+      <c r="AF19" s="100">
         <v>1003</v>
       </c>
       <c r="AG19" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="AH19" s="109">
+      <c r="AH19" s="100">
         <v>210</v>
       </c>
       <c r="AI19" s="14"/>
@@ -4345,13 +4439,13 @@
       <c r="X20" s="14"/>
       <c r="Y20" s="14"/>
       <c r="AE20" s="1"/>
-      <c r="AF20" s="109">
+      <c r="AF20" s="100">
         <v>1004</v>
       </c>
       <c r="AG20" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="AH20" s="109">
+      <c r="AH20" s="100">
         <v>210</v>
       </c>
       <c r="AI20" s="14"/>
@@ -4391,13 +4485,13 @@
       <c r="W21" s="5"/>
       <c r="X21" s="14"/>
       <c r="Y21" s="14"/>
-      <c r="AF21" s="110">
+      <c r="AF21" s="101">
         <v>5130</v>
       </c>
       <c r="AG21" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="AH21" s="110">
+      <c r="AH21" s="101">
         <v>210</v>
       </c>
       <c r="AI21" s="14"/>
@@ -7011,44 +7105,44 @@
       <c r="B89" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="F89" s="104" t="s">
+      <c r="F89" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="G89" s="105"/>
-      <c r="H89" s="104" t="s">
+      <c r="G89" s="113"/>
+      <c r="H89" s="112" t="s">
         <v>70</v>
       </c>
-      <c r="I89" s="105"/>
-      <c r="J89" s="104" t="s">
+      <c r="I89" s="113"/>
+      <c r="J89" s="112" t="s">
         <v>71</v>
       </c>
-      <c r="K89" s="105"/>
-      <c r="L89" s="104" t="s">
+      <c r="K89" s="113"/>
+      <c r="L89" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="M89" s="105"/>
-      <c r="N89" s="104" t="s">
+      <c r="M89" s="113"/>
+      <c r="N89" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="O89" s="106"/>
-      <c r="P89" s="100" t="s">
+      <c r="O89" s="114"/>
+      <c r="P89" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="Q89" s="101"/>
-      <c r="R89" s="100" t="s">
+      <c r="Q89" s="111"/>
+      <c r="R89" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="S89" s="101"/>
-      <c r="T89" s="100" t="s">
+      <c r="S89" s="111"/>
+      <c r="T89" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="U89" s="102"/>
-      <c r="V89" s="100" t="s">
+      <c r="U89" s="110"/>
+      <c r="V89" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="W89" s="101"/>
-      <c r="X89" s="103"/>
-      <c r="Y89" s="103"/>
+      <c r="W89" s="111"/>
+      <c r="X89" s="115"/>
+      <c r="Y89" s="115"/>
       <c r="Z89" s="24"/>
       <c r="AA89" s="24"/>
     </row>
@@ -9171,6 +9265,16 @@
     <sortCondition ref="B10:B79"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="P89:Q89"/>
+    <mergeCell ref="R89:S89"/>
+    <mergeCell ref="T89:U89"/>
+    <mergeCell ref="V89:W89"/>
+    <mergeCell ref="X89:Y89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="L89:M89"/>
+    <mergeCell ref="N89:O89"/>
     <mergeCell ref="T8:U8"/>
     <mergeCell ref="V8:W8"/>
     <mergeCell ref="P8:Q8"/>
@@ -9180,16 +9284,6 @@
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="N8:O8"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="L89:M89"/>
-    <mergeCell ref="N89:O89"/>
-    <mergeCell ref="P89:Q89"/>
-    <mergeCell ref="R89:S89"/>
-    <mergeCell ref="T89:U89"/>
-    <mergeCell ref="V89:W89"/>
-    <mergeCell ref="X89:Y89"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9199,6 +9293,215 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DFB419-1B8C-467B-87EE-1FBB4624B23C}">
+  <dimension ref="G6:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="44.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="8:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="8:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="120" t="s">
+        <v>286</v>
+      </c>
+      <c r="I7" s="121" t="s">
+        <v>284</v>
+      </c>
+      <c r="J7" s="122" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H8" s="131" t="s">
+        <v>287</v>
+      </c>
+      <c r="I8" s="126">
+        <v>2515</v>
+      </c>
+      <c r="J8" s="118">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="9" spans="8:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="123" t="s">
+        <v>288</v>
+      </c>
+      <c r="I9" s="127">
+        <v>2511</v>
+      </c>
+      <c r="J9" s="118">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="10" spans="8:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H10" s="124" t="s">
+        <v>289</v>
+      </c>
+      <c r="I10" s="127">
+        <v>3218</v>
+      </c>
+      <c r="J10" s="118">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H11" s="123" t="s">
+        <v>290</v>
+      </c>
+      <c r="I11" s="127">
+        <v>1003</v>
+      </c>
+      <c r="J11" s="118">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H12" s="129" t="s">
+        <v>291</v>
+      </c>
+      <c r="I12" s="127">
+        <v>1004</v>
+      </c>
+      <c r="J12" s="118">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H13" s="123" t="s">
+        <v>292</v>
+      </c>
+      <c r="I13" s="127">
+        <v>5130</v>
+      </c>
+      <c r="J13" s="118">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H14" s="129" t="s">
+        <v>291</v>
+      </c>
+      <c r="I14" s="127">
+        <v>5131</v>
+      </c>
+      <c r="J14" s="118">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H15" s="130" t="s">
+        <v>293</v>
+      </c>
+      <c r="I15" s="127">
+        <v>2510</v>
+      </c>
+      <c r="J15" s="118">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H16" s="123" t="s">
+        <v>294</v>
+      </c>
+      <c r="I16" s="127">
+        <v>1964</v>
+      </c>
+      <c r="J16" s="118">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H17" s="123" t="s">
+        <v>292</v>
+      </c>
+      <c r="I17" s="127">
+        <v>1005</v>
+      </c>
+      <c r="J17" s="118">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H18" s="130" t="s">
+        <v>295</v>
+      </c>
+      <c r="I18" s="127">
+        <v>1006</v>
+      </c>
+      <c r="J18" s="118">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H19" s="123" t="s">
+        <v>296</v>
+      </c>
+      <c r="I19" s="127">
+        <v>973</v>
+      </c>
+      <c r="J19" s="118">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H20" s="123" t="s">
+        <v>297</v>
+      </c>
+      <c r="I20" s="127">
+        <v>2509</v>
+      </c>
+      <c r="J20" s="118">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H21" s="123" t="s">
+        <v>298</v>
+      </c>
+      <c r="I21" s="127">
+        <v>2508</v>
+      </c>
+      <c r="J21" s="118">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H22" s="123" t="s">
+        <v>299</v>
+      </c>
+      <c r="I22" s="127">
+        <v>5218</v>
+      </c>
+      <c r="J22" s="118">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="8:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="125" t="s">
+        <v>300</v>
+      </c>
+      <c r="I23" s="128">
+        <v>5142</v>
+      </c>
+      <c r="J23" s="119">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82919BA3-099A-414C-AF8B-EA89BAA9CE4F}">
   <dimension ref="B1:AN133"/>
   <sheetViews>
@@ -9243,66 +9546,66 @@
   <sheetData>
     <row r="1" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="108"/>
+      <c r="G2" s="117"/>
       <c r="H2" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="J2" s="107" t="s">
+      <c r="J2" s="116" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="108"/>
+      <c r="K2" s="117"/>
       <c r="L2" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="107" t="s">
+      <c r="N2" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="O2" s="108"/>
+      <c r="O2" s="117"/>
       <c r="P2" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="R2" s="107" t="s">
+      <c r="R2" s="116" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="108"/>
+      <c r="S2" s="117"/>
       <c r="T2" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="V2" s="107" t="s">
+      <c r="V2" s="116" t="s">
         <v>88</v>
       </c>
-      <c r="W2" s="108"/>
+      <c r="W2" s="117"/>
       <c r="X2" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="Z2" s="107" t="s">
+      <c r="Z2" s="116" t="s">
         <v>90</v>
       </c>
-      <c r="AA2" s="108"/>
+      <c r="AA2" s="117"/>
       <c r="AB2" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AD2" s="107" t="s">
+      <c r="AD2" s="116" t="s">
         <v>91</v>
       </c>
-      <c r="AE2" s="108"/>
+      <c r="AE2" s="117"/>
       <c r="AF2" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AH2" s="107" t="s">
+      <c r="AH2" s="116" t="s">
         <v>92</v>
       </c>
-      <c r="AI2" s="108"/>
+      <c r="AI2" s="117"/>
       <c r="AJ2" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AL2" s="107" t="s">
+      <c r="AL2" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="AM2" s="108"/>
+      <c r="AM2" s="117"/>
       <c r="AN2" s="55" t="s">
         <v>86</v>
       </c>
@@ -11096,7 +11399,7 @@
       </c>
     </row>
     <row r="27" spans="2:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="111" t="s">
+      <c r="B27" s="102" t="s">
         <v>269</v>
       </c>
       <c r="C27" s="47" t="s">
@@ -11145,7 +11448,7 @@
       <c r="B28" s="2">
         <v>161</v>
       </c>
-      <c r="C28" s="113">
+      <c r="C28" s="104">
         <v>139</v>
       </c>
       <c r="F28" s="3">
@@ -11194,7 +11497,7 @@
       <c r="B29" s="3">
         <v>133</v>
       </c>
-      <c r="C29" s="109">
+      <c r="C29" s="100">
         <v>129</v>
       </c>
       <c r="F29" s="3">
@@ -11240,7 +11543,7 @@
       <c r="B30" s="3">
         <v>122</v>
       </c>
-      <c r="C30" s="109">
+      <c r="C30" s="100">
         <v>129</v>
       </c>
       <c r="F30" s="3">
@@ -11286,7 +11589,7 @@
       <c r="B31" s="3">
         <v>132</v>
       </c>
-      <c r="C31" s="109">
+      <c r="C31" s="100">
         <v>129</v>
       </c>
       <c r="F31" s="3">
@@ -11326,7 +11629,7 @@
       <c r="B32" s="3">
         <v>127</v>
       </c>
-      <c r="C32" s="109">
+      <c r="C32" s="100">
         <v>127</v>
       </c>
       <c r="F32" s="3">
@@ -11360,7 +11663,7 @@
       <c r="B33" s="6">
         <v>239</v>
       </c>
-      <c r="C33" s="110">
+      <c r="C33" s="101">
         <v>122</v>
       </c>
       <c r="F33" s="3">
@@ -13323,12 +13626,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D60CAF6-4CB0-4963-BE89-E20C75FEF9DA}">
   <dimension ref="H10:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13341,39 +13644,39 @@
     </row>
     <row r="13" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H14" s="117" t="s">
+      <c r="H14" s="108" t="s">
         <v>283</v>
       </c>
-      <c r="I14" s="111">
+      <c r="I14" s="102">
         <v>1</v>
       </c>
-      <c r="J14" s="114">
+      <c r="J14" s="105">
         <v>2</v>
       </c>
-      <c r="K14" s="114">
+      <c r="K14" s="105">
         <v>3</v>
       </c>
-      <c r="L14" s="114">
+      <c r="L14" s="105">
         <v>4</v>
       </c>
-      <c r="M14" s="114">
+      <c r="M14" s="105">
         <v>5</v>
       </c>
-      <c r="N14" s="114">
+      <c r="N14" s="105">
         <v>6</v>
       </c>
-      <c r="O14" s="114">
+      <c r="O14" s="105">
         <v>7</v>
       </c>
-      <c r="P14" s="114">
+      <c r="P14" s="105">
         <v>8</v>
       </c>
-      <c r="Q14" s="112">
+      <c r="Q14" s="103">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="8:17" x14ac:dyDescent="0.3">
-      <c r="H15" s="115" t="s">
+      <c r="H15" s="106" t="s">
         <v>270</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -13405,7 +13708,7 @@
       </c>
     </row>
     <row r="16" spans="8:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H16" s="116" t="s">
+      <c r="H16" s="107" t="s">
         <v>271</v>
       </c>
       <c r="I16" s="6" t="s">

</xml_diff>